<commit_message>
Zeit_angepaasst von UTC auf Berliner zeit
</commit_message>
<xml_diff>
--- a/output/Muster_Honorarrechnung-Lehrkräfte_February.xlsx
+++ b/output/Muster_Honorarrechnung-Lehrkräfte_February.xlsx
@@ -976,7 +976,7 @@
       </c>
       <c r="E23" s="47" t="inlineStr">
         <is>
-          <t>01.03.2026</t>
+          <t>28.02.2026</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       <c r="B24" s="18" t="n"/>
       <c r="C24" s="27" t="inlineStr">
         <is>
-          <t>04.02.2026 bis 01.03.2026</t>
+          <t>04.02.2026 bis 28.02.2026</t>
         </is>
       </c>
       <c r="D24" s="10" t="n"/>
@@ -1239,7 +1239,7 @@
     <row r="40">
       <c r="A40" s="44" t="inlineStr">
         <is>
-          <t>01.03.2026</t>
+          <t>28.02.2026</t>
         </is>
       </c>
       <c r="B40" s="17" t="n">

</xml_diff>

<commit_message>
env.dev und env-prod erstellt
</commit_message>
<xml_diff>
--- a/output/Muster_Honorarrechnung-Lehrkräfte_February.xlsx
+++ b/output/Muster_Honorarrechnung-Lehrkräfte_February.xlsx
@@ -976,7 +976,7 @@
       </c>
       <c r="E23" s="47" t="inlineStr">
         <is>
-          <t>28.02.2026</t>
+          <t>26.02.2026</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       <c r="B24" s="18" t="n"/>
       <c r="C24" s="27" t="inlineStr">
         <is>
-          <t>04.02.2026 bis 28.02.2026</t>
+          <t>04.02.2026 bis 26.02.2026</t>
         </is>
       </c>
       <c r="D24" s="10" t="n"/>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C33" s="26" t="inlineStr">
         <is>
-          <t>Unterricht</t>
+          <t>Unterricht ASA 8</t>
         </is>
       </c>
       <c r="D33" s="16" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C35" s="26" t="inlineStr">
         <is>
-          <t>Unterricht</t>
+          <t>Unterricht ASA 8</t>
         </is>
       </c>
       <c r="D35" s="16" t="n">
@@ -1151,15 +1151,15 @@
     <row r="36">
       <c r="A36" s="44" t="inlineStr">
         <is>
-          <t>18.02.2026</t>
+          <t>13.02.2026</t>
         </is>
       </c>
       <c r="B36" s="25" t="n">
-        <v>0.75</v>
+        <v>3.25</v>
       </c>
       <c r="C36" s="26" t="inlineStr">
         <is>
-          <t>Vorbereitung für Unterricht: 0,75 Stunden</t>
+          <t>Unterricht ASA 9 Vertretung</t>
         </is>
       </c>
       <c r="D36" s="16" t="n">
@@ -1173,15 +1173,15 @@
     <row r="37">
       <c r="A37" s="44" t="inlineStr">
         <is>
-          <t>19.02.2026</t>
+          <t>16.02.2026</t>
         </is>
       </c>
       <c r="B37" s="25" t="n">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="C37" s="26" t="inlineStr">
         <is>
-          <t>Unterricht</t>
+          <t>Vorbereitung für Unterricht: 0,75 Stunden</t>
         </is>
       </c>
       <c r="D37" s="16" t="n">
@@ -1195,15 +1195,15 @@
     <row r="38">
       <c r="A38" s="44" t="inlineStr">
         <is>
-          <t>25.02.2026</t>
+          <t>17.02.2026</t>
         </is>
       </c>
       <c r="B38" s="25" t="n">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="C38" s="26" t="inlineStr">
         <is>
-          <t>Vorbereitung für Unterricht: 0,75 Stunden</t>
+          <t>Unterricht ASA 8</t>
         </is>
       </c>
       <c r="D38" s="16" t="n">
@@ -1217,15 +1217,15 @@
     <row r="39">
       <c r="A39" s="44" t="inlineStr">
         <is>
-          <t>26.02.2026</t>
+          <t>18.02.2026</t>
         </is>
       </c>
       <c r="B39" s="17" t="n">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="C39" s="26" t="inlineStr">
         <is>
-          <t>Unterricht</t>
+          <t>Vorbereitung für Unterricht: 0,75 Stunden</t>
         </is>
       </c>
       <c r="D39" s="16" t="n">
@@ -1239,13 +1239,17 @@
     <row r="40">
       <c r="A40" s="44" t="inlineStr">
         <is>
-          <t>28.02.2026</t>
+          <t>19.02.2026</t>
         </is>
       </c>
       <c r="B40" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="15" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C40" s="15" t="inlineStr">
+        <is>
+          <t>Unterricht ASA 8</t>
+        </is>
+      </c>
       <c r="D40" s="16" t="n">
         <v>19</v>
       </c>
@@ -1255,20 +1259,44 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="44" t="n"/>
-      <c r="B41" s="17" t="n"/>
-      <c r="C41" s="15" t="n"/>
-      <c r="D41" s="16" t="n"/>
+      <c r="A41" s="44" t="inlineStr">
+        <is>
+          <t>25.02.2026</t>
+        </is>
+      </c>
+      <c r="B41" s="17" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C41" s="15" t="inlineStr">
+        <is>
+          <t>Vorbereitung für Unterricht: 0,75 Stunden</t>
+        </is>
+      </c>
+      <c r="D41" s="16" t="n">
+        <v>19</v>
+      </c>
       <c r="E41" s="37">
         <f>ROUND(B41*$D$32,2)</f>
         <v/>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="44" t="n"/>
-      <c r="B42" s="17" t="n"/>
-      <c r="C42" s="15" t="n"/>
-      <c r="D42" s="16" t="n"/>
+      <c r="A42" s="44" t="inlineStr">
+        <is>
+          <t>26.02.2026</t>
+        </is>
+      </c>
+      <c r="B42" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" s="15" t="inlineStr">
+        <is>
+          <t>Unterricht ASA 8</t>
+        </is>
+      </c>
+      <c r="D42" s="16" t="n">
+        <v>19</v>
+      </c>
       <c r="E42" s="37">
         <f>ROUND(B42*$D$32,2)</f>
         <v/>

</xml_diff>